<commit_message>
fixed the column width problem by specifiying width manually
</commit_message>
<xml_diff>
--- a/LS_rating_apr.xlsx
+++ b/LS_rating_apr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaimin Khaw\Desktop\credit-rating-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DEED4EC-3AAA-4DD5-AAF8-07D4A8E1EED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD9E02B1-D2F3-441E-90A4-112B86A4FC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ratings" sheetId="1" r:id="rId1"/>
@@ -727,7 +727,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -745,6 +745,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5492,7 +5493,7 @@
   <dimension ref="A1:I139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A141" sqref="A141"/>
+      <selection activeCell="I146" sqref="I146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6347,13 +6348,13 @@
       <c r="A29" t="s">
         <v>75</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="9">
         <v>3.6666666666666679</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="9">
         <v>6.5350300207615941</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="9">
         <v>5.8755298865392529</v>
       </c>
       <c r="E29" s="6">
@@ -6366,7 +6367,7 @@
       <c r="G29">
         <v>-2.75</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="9">
         <v>3.1255298865392529</v>
       </c>
       <c r="I29" t="s">
@@ -7157,13 +7158,13 @@
       <c r="A56" t="s">
         <v>113</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="9">
         <v>18.333333333333329</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="9">
         <v>19.14169073459334</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="9">
         <v>19.524027891716411</v>
       </c>
       <c r="E56" s="6">
@@ -7176,7 +7177,7 @@
       <c r="G56">
         <v>-1.5</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="9">
         <v>18.024027891716411</v>
       </c>
       <c r="I56" t="s">
@@ -7277,13 +7278,13 @@
       <c r="A60" t="s">
         <v>117</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="9">
         <v>18.333333333333329</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="9">
         <v>15.911103201564361</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="9">
         <v>16.261999921398441</v>
       </c>
       <c r="E60" s="6">
@@ -7296,7 +7297,7 @@
       <c r="G60">
         <v>0.2</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="9">
         <v>16.461999921398441</v>
       </c>
       <c r="I60" t="s">
@@ -7607,13 +7608,13 @@
       <c r="A71" t="s">
         <v>129</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="9">
         <v>4</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="9">
         <v>6.0635521333406546</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="9">
         <v>6.4773497220357958</v>
       </c>
       <c r="E71" s="6">
@@ -7626,7 +7627,7 @@
       <c r="G71">
         <v>0</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="9">
         <v>6.4773497220357958</v>
       </c>
       <c r="I71" t="s">
@@ -8168,13 +8169,13 @@
       <c r="A90" t="s">
         <v>149</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="9">
         <v>6.3333333333333321</v>
       </c>
-      <c r="C90">
+      <c r="C90" s="9">
         <v>7.0383148623084946</v>
       </c>
-      <c r="D90">
+      <c r="D90" s="9">
         <v>7.5150603654213031</v>
       </c>
       <c r="E90" s="6">
@@ -8187,7 +8188,7 @@
       <c r="G90">
         <v>-1</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="9">
         <v>6.5150603654213031</v>
       </c>
       <c r="I90" t="s">
@@ -8198,13 +8199,13 @@
       <c r="A91" t="s">
         <v>150</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="9">
         <v>10.66666666666667</v>
       </c>
-      <c r="C91">
+      <c r="C91" s="9">
         <v>9.8225052294429851</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="9">
         <v>10.11020208150434</v>
       </c>
       <c r="E91" s="6">
@@ -8217,7 +8218,7 @@
       <c r="G91">
         <v>1.5</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="9">
         <v>11.61020208150434</v>
       </c>
       <c r="I91" t="s">
@@ -8438,13 +8439,13 @@
       <c r="A99" t="s">
         <v>161</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="9">
         <v>7.3333333333333339</v>
       </c>
-      <c r="C99">
+      <c r="C99" s="9">
         <v>7.1308446545654078</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="9">
         <v>8.1673569381872326</v>
       </c>
       <c r="E99" s="6">
@@ -8457,7 +8458,7 @@
       <c r="G99">
         <v>0.5</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="9">
         <v>8.6673569381872326</v>
       </c>
       <c r="I99" t="s">
@@ -8528,13 +8529,13 @@
       <c r="A102" t="s">
         <v>164</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="9">
         <v>6.5</v>
       </c>
-      <c r="C102">
+      <c r="C102" s="9">
         <v>7.9619617802781271</v>
       </c>
-      <c r="D102">
+      <c r="D102" s="9">
         <v>7.5506333624641204</v>
       </c>
       <c r="E102" s="6">
@@ -8547,7 +8548,7 @@
       <c r="G102">
         <v>-1</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="9">
         <v>6.5506333624641204</v>
       </c>
       <c r="I102" t="s">
@@ -9458,13 +9459,13 @@
       <c r="A133" t="s">
         <v>195</v>
       </c>
-      <c r="B133">
+      <c r="B133" s="9">
         <v>8.6666666666666661</v>
       </c>
-      <c r="C133">
+      <c r="C133" s="9">
         <v>10.73479249215913</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="9">
         <v>10.406829779554879</v>
       </c>
       <c r="E133" s="6">
@@ -9477,7 +9478,7 @@
       <c r="G133">
         <v>-1.25</v>
       </c>
-      <c r="H133">
+      <c r="H133" s="9">
         <v>9.1568297795548794</v>
       </c>
       <c r="I133" t="s">

</xml_diff>